<commit_message>
excel file for lab1
</commit_message>
<xml_diff>
--- a/ise301_modopt2_lab1.xlsx
+++ b/ise301_modopt2_lab1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\serhan.aydin\Documents\teaching\op_res_II\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\serhan.aydin\Documents\GitHub\ise301_modopt2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8C64E61E-58CF-4ABE-856C-9353402D4B5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{551B516C-90E2-45C3-A218-C92BE28014CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="7" xr2:uid="{73B21749-A357-4946-A02C-9A1A428E9DFD}"/>
   </bookViews>
@@ -1642,7 +1642,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>